<commit_message>
started on toolbar, bug fixes to territory writer, and updates to excel sample
</commit_message>
<xml_diff>
--- a/templates/simple.xlsx
+++ b/templates/simple.xlsx
@@ -192,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -441,11 +441,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -517,38 +550,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,38 +634,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,7 +947,7 @@
   <dimension ref="A1:DK106"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="AL16" sqref="AL16"/>
+      <selection activeCell="AV9" sqref="AV9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,46 +957,49 @@
     <col min="6" max="13" width="3.28515625" style="2"/>
     <col min="14" max="16" width="3.28515625" style="2" customWidth="1"/>
     <col min="17" max="20" width="3.28515625" style="2"/>
-    <col min="21" max="21" width="3.28515625" style="28" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="26" customWidth="1"/>
     <col min="22" max="22" width="0.5703125" style="2" customWidth="1"/>
     <col min="23" max="27" width="3.28515625" style="2"/>
     <col min="28" max="28" width="3" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="3.28515625" style="2"/>
+    <col min="29" max="35" width="3.28515625" style="2"/>
+    <col min="36" max="42" width="3.28515625" style="2" customWidth="1"/>
+    <col min="43" max="43" width="3.140625" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="3.28515625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:115" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="36" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="38" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="36" t="s">
+      <c r="P1" s="46"/>
+      <c r="Q1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="36"/>
+      <c r="R1" s="44"/>
       <c r="S1" s="16" t="s">
         <v>12</v>
       </c>
@@ -952,39 +1009,39 @@
       <c r="U1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="V1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
       <c r="Z1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AA1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="37" t="s">
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="36" t="s">
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="38" t="s">
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="44"/>
+      <c r="AK1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="36" t="s">
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AN1" s="36"/>
+      <c r="AN1" s="44"/>
       <c r="AO1" s="16" t="s">
         <v>12</v>
       </c>
@@ -1068,98 +1125,98 @@
       <c r="DK1" s="2"/>
     </row>
     <row r="2" spans="1:115" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="41" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-      <c r="AQ2" s="39"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
     </row>
     <row r="3" spans="1:115" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="42"/>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="42"/>
-      <c r="AM3" s="42"/>
-      <c r="AN3" s="42"/>
-      <c r="AO3" s="42"/>
-      <c r="AP3" s="42"/>
-      <c r="AQ3" s="42"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50"/>
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AP3" s="50"/>
+      <c r="AQ3" s="50"/>
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
       <c r="AT3" s="2"/>
@@ -1234,21 +1291,21 @@
       <c r="DK3" s="2"/>
     </row>
     <row r="4" spans="1:115" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
@@ -1257,22 +1314,22 @@
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
       <c r="U4" s="13"/>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
+      <c r="AE4" s="54"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="54"/>
+      <c r="AI4" s="55"/>
       <c r="AJ4" s="13"/>
       <c r="AK4" s="13"/>
       <c r="AL4" s="13"/>
@@ -1354,21 +1411,21 @@
       <c r="DK4" s="2"/>
     </row>
     <row r="5" spans="1:115" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -1377,28 +1434,29 @@
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
-      <c r="V5" s="31" t="s">
+      <c r="V5" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
+      <c r="W5" s="60"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="53"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="55"/>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="6"/>
       <c r="AL5" s="6"/>
       <c r="AM5" s="6"/>
       <c r="AN5" s="6"/>
       <c r="AP5" s="6"/>
+      <c r="AQ5" s="28"/>
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
@@ -1473,23 +1531,23 @@
       <c r="DK5" s="2"/>
     </row>
     <row r="6" spans="1:115" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="51"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="62"/>
       <c r="N6" s="8" t="s">
         <v>1</v>
       </c>
@@ -1515,23 +1573,23 @@
         <v>8</v>
       </c>
       <c r="V6" s="17"/>
-      <c r="W6" s="47" t="s">
+      <c r="W6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="47"/>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="49" t="s">
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="AC6" s="50"/>
-      <c r="AD6" s="50"/>
-      <c r="AE6" s="50"/>
-      <c r="AF6" s="50"/>
-      <c r="AG6" s="50"/>
-      <c r="AH6" s="50"/>
-      <c r="AI6" s="50"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="35"/>
+      <c r="AE6" s="35"/>
+      <c r="AF6" s="35"/>
+      <c r="AG6" s="35"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="35"/>
       <c r="AJ6" s="8" t="s">
         <v>1</v>
       </c>
@@ -1550,10 +1608,10 @@
       <c r="AO6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AP6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AQ6" s="29" t="s">
         <v>8</v>
       </c>
       <c r="AR6" s="3"/>
@@ -1630,36 +1688,35 @@
       <c r="DK6" s="3"/>
     </row>
     <row r="7" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="54"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="57"/>
       <c r="T7" s="11"/>
       <c r="V7" s="18"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="46"/>
-      <c r="AD7" s="46"/>
-      <c r="AE7" s="46"/>
-      <c r="AF7" s="46"/>
-      <c r="AG7" s="46"/>
-      <c r="AH7" s="46"/>
-      <c r="AI7" s="46"/>
-      <c r="AJ7" s="55"/>
-      <c r="AQ7" s="20"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="33"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="37"/>
+      <c r="AD7" s="37"/>
+      <c r="AE7" s="37"/>
+      <c r="AF7" s="37"/>
+      <c r="AG7" s="37"/>
+      <c r="AH7" s="37"/>
+      <c r="AI7" s="37"/>
+      <c r="AQ7" s="11"/>
       <c r="AR7" s="3"/>
       <c r="AS7" s="3"/>
       <c r="AT7" s="3"/>
@@ -1734,35 +1791,34 @@
       <c r="DK7" s="3"/>
     </row>
     <row r="8" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="54"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="57"/>
       <c r="T8" s="11"/>
       <c r="V8" s="18"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="34"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="45"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="46"/>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="46"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="55"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="33"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="37"/>
+      <c r="AD8" s="37"/>
+      <c r="AE8" s="37"/>
+      <c r="AF8" s="37"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="37"/>
+      <c r="AI8" s="37"/>
       <c r="AQ8" s="20"/>
       <c r="AR8" s="3"/>
       <c r="AS8" s="3"/>
@@ -1838,35 +1894,34 @@
       <c r="DK8" s="3"/>
     </row>
     <row r="9" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="54"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="57"/>
       <c r="T9" s="11"/>
       <c r="V9" s="18"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="34"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="45"/>
-      <c r="AC9" s="46"/>
-      <c r="AD9" s="46"/>
-      <c r="AE9" s="46"/>
-      <c r="AF9" s="46"/>
-      <c r="AG9" s="46"/>
-      <c r="AH9" s="46"/>
-      <c r="AI9" s="46"/>
-      <c r="AJ9" s="55"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="33"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="37"/>
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="37"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" s="37"/>
       <c r="AQ9" s="20"/>
       <c r="AR9" s="3"/>
       <c r="AS9" s="3"/>
@@ -1942,35 +1997,34 @@
       <c r="DK9" s="3"/>
     </row>
     <row r="10" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="57"/>
       <c r="T10" s="11"/>
       <c r="V10" s="18"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="45"/>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="46"/>
-      <c r="AH10" s="46"/>
-      <c r="AI10" s="46"/>
-      <c r="AJ10" s="55"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="37"/>
+      <c r="AD10" s="37"/>
+      <c r="AE10" s="37"/>
+      <c r="AF10" s="37"/>
+      <c r="AG10" s="37"/>
+      <c r="AH10" s="37"/>
+      <c r="AI10" s="37"/>
       <c r="AQ10" s="20"/>
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
@@ -2046,35 +2100,34 @@
       <c r="DK10" s="3"/>
     </row>
     <row r="11" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="54"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="57"/>
       <c r="T11" s="11"/>
       <c r="V11" s="18"/>
-      <c r="W11" s="34"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="35"/>
-      <c r="AB11" s="45"/>
-      <c r="AC11" s="46"/>
-      <c r="AD11" s="46"/>
-      <c r="AE11" s="46"/>
-      <c r="AF11" s="46"/>
-      <c r="AG11" s="46"/>
-      <c r="AH11" s="46"/>
-      <c r="AI11" s="46"/>
-      <c r="AJ11" s="55"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="37"/>
+      <c r="AD11" s="37"/>
+      <c r="AE11" s="37"/>
+      <c r="AF11" s="37"/>
+      <c r="AG11" s="37"/>
+      <c r="AH11" s="37"/>
+      <c r="AI11" s="37"/>
       <c r="AQ11" s="20"/>
       <c r="AR11" s="3"/>
       <c r="AS11" s="3"/>
@@ -2150,35 +2203,34 @@
       <c r="DK11" s="3"/>
     </row>
     <row r="12" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="54"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="57"/>
       <c r="T12" s="11"/>
       <c r="V12" s="18"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="45"/>
-      <c r="AC12" s="46"/>
-      <c r="AD12" s="46"/>
-      <c r="AE12" s="46"/>
-      <c r="AF12" s="46"/>
-      <c r="AG12" s="46"/>
-      <c r="AH12" s="46"/>
-      <c r="AI12" s="46"/>
-      <c r="AJ12" s="55"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="37"/>
+      <c r="AE12" s="37"/>
+      <c r="AF12" s="37"/>
+      <c r="AG12" s="37"/>
+      <c r="AH12" s="37"/>
+      <c r="AI12" s="37"/>
       <c r="AQ12" s="20"/>
       <c r="AR12" s="3"/>
       <c r="AS12" s="3"/>
@@ -2254,35 +2306,34 @@
       <c r="DK12" s="3"/>
     </row>
     <row r="13" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="54"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="57"/>
       <c r="T13" s="11"/>
       <c r="V13" s="18"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="45"/>
-      <c r="AC13" s="46"/>
-      <c r="AD13" s="46"/>
-      <c r="AE13" s="46"/>
-      <c r="AF13" s="46"/>
-      <c r="AG13" s="46"/>
-      <c r="AH13" s="46"/>
-      <c r="AI13" s="46"/>
-      <c r="AJ13" s="55"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37"/>
+      <c r="AI13" s="37"/>
       <c r="AQ13" s="20"/>
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
@@ -2358,35 +2409,34 @@
       <c r="DK13" s="3"/>
     </row>
     <row r="14" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="54"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="57"/>
       <c r="T14" s="11"/>
       <c r="V14" s="18"/>
-      <c r="W14" s="34"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="45"/>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46"/>
-      <c r="AE14" s="46"/>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="46"/>
-      <c r="AI14" s="46"/>
-      <c r="AJ14" s="55"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="37"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
+      <c r="AH14" s="37"/>
+      <c r="AI14" s="37"/>
       <c r="AQ14" s="20"/>
       <c r="AR14" s="3"/>
       <c r="AS14" s="3"/>
@@ -2462,35 +2512,34 @@
       <c r="DK14" s="3"/>
     </row>
     <row r="15" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="54"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="57"/>
       <c r="T15" s="11"/>
       <c r="V15" s="18"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="45"/>
-      <c r="AC15" s="46"/>
-      <c r="AD15" s="46"/>
-      <c r="AE15" s="46"/>
-      <c r="AF15" s="46"/>
-      <c r="AG15" s="46"/>
-      <c r="AH15" s="46"/>
-      <c r="AI15" s="46"/>
-      <c r="AJ15" s="55"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="33"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="37"/>
+      <c r="AD15" s="37"/>
+      <c r="AE15" s="37"/>
+      <c r="AF15" s="37"/>
+      <c r="AG15" s="37"/>
+      <c r="AH15" s="37"/>
+      <c r="AI15" s="37"/>
       <c r="AQ15" s="20"/>
       <c r="AR15" s="3"/>
       <c r="AS15" s="3"/>
@@ -2566,35 +2615,34 @@
       <c r="DK15" s="3"/>
     </row>
     <row r="16" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="54"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="57"/>
       <c r="T16" s="11"/>
       <c r="V16" s="19"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="34"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="46"/>
-      <c r="AD16" s="46"/>
-      <c r="AE16" s="46"/>
-      <c r="AF16" s="46"/>
-      <c r="AG16" s="46"/>
-      <c r="AH16" s="46"/>
-      <c r="AI16" s="46"/>
-      <c r="AJ16" s="55"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="37"/>
+      <c r="AE16" s="37"/>
+      <c r="AF16" s="37"/>
+      <c r="AG16" s="37"/>
+      <c r="AH16" s="37"/>
+      <c r="AI16" s="37"/>
       <c r="AQ16" s="20"/>
       <c r="AR16" s="3"/>
       <c r="AS16" s="3"/>
@@ -2670,35 +2718,34 @@
       <c r="DK16" s="3"/>
     </row>
     <row r="17" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="54"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="57"/>
       <c r="T17" s="11"/>
       <c r="V17" s="18"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="34"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="45"/>
-      <c r="AC17" s="46"/>
-      <c r="AD17" s="46"/>
-      <c r="AE17" s="46"/>
-      <c r="AF17" s="46"/>
-      <c r="AG17" s="46"/>
-      <c r="AH17" s="46"/>
-      <c r="AI17" s="46"/>
-      <c r="AJ17" s="55"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37"/>
+      <c r="AI17" s="37"/>
       <c r="AQ17" s="20"/>
       <c r="AR17" s="3"/>
       <c r="AS17" s="3"/>
@@ -2774,35 +2821,34 @@
       <c r="DK17" s="3"/>
     </row>
     <row r="18" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="54"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="57"/>
       <c r="T18" s="11"/>
       <c r="V18" s="18"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="45"/>
-      <c r="AC18" s="46"/>
-      <c r="AD18" s="46"/>
-      <c r="AE18" s="46"/>
-      <c r="AF18" s="46"/>
-      <c r="AG18" s="46"/>
-      <c r="AH18" s="46"/>
-      <c r="AI18" s="46"/>
-      <c r="AJ18" s="55"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="37"/>
+      <c r="AF18" s="37"/>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
       <c r="AQ18" s="20"/>
       <c r="AR18" s="3"/>
       <c r="AS18" s="3"/>
@@ -2878,35 +2924,34 @@
       <c r="DK18" s="3"/>
     </row>
     <row r="19" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="54"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="57"/>
       <c r="T19" s="11"/>
       <c r="V19" s="18"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="34"/>
-      <c r="AA19" s="35"/>
-      <c r="AB19" s="45"/>
-      <c r="AC19" s="46"/>
-      <c r="AD19" s="46"/>
-      <c r="AE19" s="46"/>
-      <c r="AF19" s="46"/>
-      <c r="AG19" s="46"/>
-      <c r="AH19" s="46"/>
-      <c r="AI19" s="46"/>
-      <c r="AJ19" s="55"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="33"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="37"/>
+      <c r="AD19" s="37"/>
+      <c r="AE19" s="37"/>
+      <c r="AF19" s="37"/>
+      <c r="AG19" s="37"/>
+      <c r="AH19" s="37"/>
+      <c r="AI19" s="37"/>
       <c r="AQ19" s="20"/>
       <c r="AR19" s="3"/>
       <c r="AS19" s="3"/>
@@ -2982,35 +3027,34 @@
       <c r="DK19" s="3"/>
     </row>
     <row r="20" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="54"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="57"/>
       <c r="T20" s="11"/>
       <c r="V20" s="18"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="35"/>
-      <c r="AB20" s="45"/>
-      <c r="AC20" s="46"/>
-      <c r="AD20" s="46"/>
-      <c r="AE20" s="46"/>
-      <c r="AF20" s="46"/>
-      <c r="AG20" s="46"/>
-      <c r="AH20" s="46"/>
-      <c r="AI20" s="46"/>
-      <c r="AJ20" s="55"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="37"/>
+      <c r="AD20" s="37"/>
+      <c r="AE20" s="37"/>
+      <c r="AF20" s="37"/>
+      <c r="AG20" s="37"/>
+      <c r="AH20" s="37"/>
+      <c r="AI20" s="37"/>
       <c r="AQ20" s="20"/>
       <c r="AR20" s="3"/>
       <c r="AS20" s="3"/>
@@ -3086,35 +3130,34 @@
       <c r="DK20" s="3"/>
     </row>
     <row r="21" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="54"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="57"/>
       <c r="T21" s="11"/>
       <c r="V21" s="18"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="34"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="45"/>
-      <c r="AC21" s="46"/>
-      <c r="AD21" s="46"/>
-      <c r="AE21" s="46"/>
-      <c r="AF21" s="46"/>
-      <c r="AG21" s="46"/>
-      <c r="AH21" s="46"/>
-      <c r="AI21" s="46"/>
-      <c r="AJ21" s="55"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+      <c r="AA21" s="33"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="37"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AF21" s="37"/>
+      <c r="AG21" s="37"/>
+      <c r="AH21" s="37"/>
+      <c r="AI21" s="37"/>
       <c r="AQ21" s="20"/>
       <c r="AR21" s="3"/>
       <c r="AS21" s="3"/>
@@ -3190,35 +3233,34 @@
       <c r="DK21" s="3"/>
     </row>
     <row r="22" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="54"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="57"/>
       <c r="T22" s="11"/>
       <c r="V22" s="18"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="34"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="45"/>
-      <c r="AC22" s="46"/>
-      <c r="AD22" s="46"/>
-      <c r="AE22" s="46"/>
-      <c r="AF22" s="46"/>
-      <c r="AG22" s="46"/>
-      <c r="AH22" s="46"/>
-      <c r="AI22" s="46"/>
-      <c r="AJ22" s="55"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
       <c r="AQ22" s="20"/>
       <c r="AR22" s="3"/>
       <c r="AS22" s="3"/>
@@ -3294,35 +3336,34 @@
       <c r="DK22" s="3"/>
     </row>
     <row r="23" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="54"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="57"/>
       <c r="T23" s="11"/>
       <c r="V23" s="18"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
-      <c r="Z23" s="34"/>
-      <c r="AA23" s="35"/>
-      <c r="AB23" s="45"/>
-      <c r="AC23" s="46"/>
-      <c r="AD23" s="46"/>
-      <c r="AE23" s="46"/>
-      <c r="AF23" s="46"/>
-      <c r="AG23" s="46"/>
-      <c r="AH23" s="46"/>
-      <c r="AI23" s="46"/>
-      <c r="AJ23" s="55"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="33"/>
+      <c r="AB23" s="36"/>
+      <c r="AC23" s="37"/>
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="37"/>
+      <c r="AF23" s="37"/>
+      <c r="AG23" s="37"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
       <c r="AQ23" s="20"/>
       <c r="AR23" s="3"/>
       <c r="AS23" s="3"/>
@@ -3398,35 +3439,34 @@
       <c r="DK23" s="3"/>
     </row>
     <row r="24" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="54"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="57"/>
       <c r="T24" s="11"/>
       <c r="V24" s="18"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="34"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="35"/>
-      <c r="AB24" s="45"/>
-      <c r="AC24" s="46"/>
-      <c r="AD24" s="46"/>
-      <c r="AE24" s="46"/>
-      <c r="AF24" s="46"/>
-      <c r="AG24" s="46"/>
-      <c r="AH24" s="46"/>
-      <c r="AI24" s="46"/>
-      <c r="AJ24" s="55"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="32"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="36"/>
+      <c r="AC24" s="37"/>
+      <c r="AD24" s="37"/>
+      <c r="AE24" s="37"/>
+      <c r="AF24" s="37"/>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
       <c r="AQ24" s="20"/>
       <c r="AR24" s="3"/>
       <c r="AS24" s="3"/>
@@ -3502,35 +3542,34 @@
       <c r="DK24" s="3"/>
     </row>
     <row r="25" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="54"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="57"/>
       <c r="T25" s="11"/>
       <c r="V25" s="18"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="35"/>
-      <c r="AB25" s="45"/>
-      <c r="AC25" s="46"/>
-      <c r="AD25" s="46"/>
-      <c r="AE25" s="46"/>
-      <c r="AF25" s="46"/>
-      <c r="AG25" s="46"/>
-      <c r="AH25" s="46"/>
-      <c r="AI25" s="46"/>
-      <c r="AJ25" s="55"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="33"/>
+      <c r="AB25" s="36"/>
+      <c r="AC25" s="37"/>
+      <c r="AD25" s="37"/>
+      <c r="AE25" s="37"/>
+      <c r="AF25" s="37"/>
+      <c r="AG25" s="37"/>
+      <c r="AH25" s="37"/>
+      <c r="AI25" s="37"/>
       <c r="AQ25" s="20"/>
       <c r="AR25" s="3"/>
       <c r="AS25" s="3"/>
@@ -3606,35 +3645,34 @@
       <c r="DK25" s="3"/>
     </row>
     <row r="26" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="54"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="57"/>
       <c r="T26" s="11"/>
       <c r="V26" s="18"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="34"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="35"/>
-      <c r="AB26" s="45"/>
-      <c r="AC26" s="46"/>
-      <c r="AD26" s="46"/>
-      <c r="AE26" s="46"/>
-      <c r="AF26" s="46"/>
-      <c r="AG26" s="46"/>
-      <c r="AH26" s="46"/>
-      <c r="AI26" s="46"/>
-      <c r="AJ26" s="55"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="32"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="36"/>
+      <c r="AC26" s="37"/>
+      <c r="AD26" s="37"/>
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="37"/>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="37"/>
+      <c r="AI26" s="37"/>
       <c r="AQ26" s="20"/>
       <c r="AR26" s="3"/>
       <c r="AS26" s="3"/>
@@ -3710,35 +3748,34 @@
       <c r="DK26" s="3"/>
     </row>
     <row r="27" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="54"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="57"/>
       <c r="T27" s="11"/>
       <c r="V27" s="18"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="35"/>
-      <c r="AB27" s="45"/>
-      <c r="AC27" s="46"/>
-      <c r="AD27" s="46"/>
-      <c r="AE27" s="46"/>
-      <c r="AF27" s="46"/>
-      <c r="AG27" s="46"/>
-      <c r="AH27" s="46"/>
-      <c r="AI27" s="46"/>
-      <c r="AJ27" s="55"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="32"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="36"/>
+      <c r="AC27" s="37"/>
+      <c r="AD27" s="37"/>
+      <c r="AE27" s="37"/>
+      <c r="AF27" s="37"/>
+      <c r="AG27" s="37"/>
+      <c r="AH27" s="37"/>
+      <c r="AI27" s="37"/>
       <c r="AQ27" s="20"/>
       <c r="AR27" s="3"/>
       <c r="AS27" s="3"/>
@@ -3814,35 +3851,34 @@
       <c r="DK27" s="3"/>
     </row>
     <row r="28" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="54"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="57"/>
       <c r="T28" s="11"/>
       <c r="V28" s="18"/>
-      <c r="W28" s="34"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="35"/>
-      <c r="AB28" s="45"/>
-      <c r="AC28" s="46"/>
-      <c r="AD28" s="46"/>
-      <c r="AE28" s="46"/>
-      <c r="AF28" s="46"/>
-      <c r="AG28" s="46"/>
-      <c r="AH28" s="46"/>
-      <c r="AI28" s="46"/>
-      <c r="AJ28" s="55"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="32"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="36"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="37"/>
+      <c r="AF28" s="37"/>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
       <c r="AQ28" s="20"/>
       <c r="AR28" s="3"/>
       <c r="AS28" s="3"/>
@@ -3918,35 +3954,34 @@
       <c r="DK28" s="3"/>
     </row>
     <row r="29" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="54"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="57"/>
       <c r="T29" s="11"/>
       <c r="V29" s="18"/>
-      <c r="W29" s="34"/>
-      <c r="X29" s="34"/>
-      <c r="Y29" s="34"/>
-      <c r="Z29" s="34"/>
-      <c r="AA29" s="35"/>
-      <c r="AB29" s="45"/>
-      <c r="AC29" s="46"/>
-      <c r="AD29" s="46"/>
-      <c r="AE29" s="46"/>
-      <c r="AF29" s="46"/>
-      <c r="AG29" s="46"/>
-      <c r="AH29" s="46"/>
-      <c r="AI29" s="46"/>
-      <c r="AJ29" s="55"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="36"/>
+      <c r="AC29" s="37"/>
+      <c r="AD29" s="37"/>
+      <c r="AE29" s="37"/>
+      <c r="AF29" s="37"/>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="37"/>
+      <c r="AI29" s="37"/>
       <c r="AQ29" s="20"/>
       <c r="AR29" s="3"/>
       <c r="AS29" s="3"/>
@@ -4022,35 +4057,34 @@
       <c r="DK29" s="3"/>
     </row>
     <row r="30" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="54"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="57"/>
       <c r="T30" s="11"/>
       <c r="V30" s="18"/>
-      <c r="W30" s="34"/>
-      <c r="X30" s="34"/>
-      <c r="Y30" s="34"/>
-      <c r="Z30" s="34"/>
-      <c r="AA30" s="35"/>
-      <c r="AB30" s="45"/>
-      <c r="AC30" s="46"/>
-      <c r="AD30" s="46"/>
-      <c r="AE30" s="46"/>
-      <c r="AF30" s="46"/>
-      <c r="AG30" s="46"/>
-      <c r="AH30" s="46"/>
-      <c r="AI30" s="46"/>
-      <c r="AJ30" s="55"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="37"/>
+      <c r="AD30" s="37"/>
+      <c r="AE30" s="37"/>
+      <c r="AF30" s="37"/>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="37"/>
       <c r="AQ30" s="20"/>
       <c r="AR30" s="3"/>
       <c r="AS30" s="3"/>
@@ -4126,35 +4160,34 @@
       <c r="DK30" s="3"/>
     </row>
     <row r="31" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="54"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="57"/>
       <c r="T31" s="11"/>
       <c r="V31" s="18"/>
-      <c r="W31" s="34"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="34"/>
-      <c r="Z31" s="34"/>
-      <c r="AA31" s="35"/>
-      <c r="AB31" s="45"/>
-      <c r="AC31" s="46"/>
-      <c r="AD31" s="46"/>
-      <c r="AE31" s="46"/>
-      <c r="AF31" s="46"/>
-      <c r="AG31" s="46"/>
-      <c r="AH31" s="46"/>
-      <c r="AI31" s="46"/>
-      <c r="AJ31" s="55"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="33"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="37"/>
+      <c r="AD31" s="37"/>
+      <c r="AE31" s="37"/>
+      <c r="AF31" s="37"/>
+      <c r="AG31" s="37"/>
+      <c r="AH31" s="37"/>
+      <c r="AI31" s="37"/>
       <c r="AQ31" s="20"/>
       <c r="AR31" s="3"/>
       <c r="AS31" s="3"/>
@@ -4230,35 +4263,34 @@
       <c r="DK31" s="3"/>
     </row>
     <row r="32" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="54"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="57"/>
       <c r="T32" s="11"/>
       <c r="V32" s="18"/>
-      <c r="W32" s="34"/>
-      <c r="X32" s="34"/>
-      <c r="Y32" s="34"/>
-      <c r="Z32" s="34"/>
-      <c r="AA32" s="35"/>
-      <c r="AB32" s="45"/>
-      <c r="AC32" s="46"/>
-      <c r="AD32" s="46"/>
-      <c r="AE32" s="46"/>
-      <c r="AF32" s="46"/>
-      <c r="AG32" s="46"/>
-      <c r="AH32" s="46"/>
-      <c r="AI32" s="46"/>
-      <c r="AJ32" s="55"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="33"/>
+      <c r="AB32" s="36"/>
+      <c r="AC32" s="37"/>
+      <c r="AD32" s="37"/>
+      <c r="AE32" s="37"/>
+      <c r="AF32" s="37"/>
+      <c r="AG32" s="37"/>
+      <c r="AH32" s="37"/>
+      <c r="AI32" s="37"/>
       <c r="AQ32" s="20"/>
       <c r="AR32" s="3"/>
       <c r="AS32" s="3"/>
@@ -4334,35 +4366,34 @@
       <c r="DK32" s="3"/>
     </row>
     <row r="33" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="54"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="57"/>
       <c r="T33" s="11"/>
       <c r="V33" s="18"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="35"/>
-      <c r="AB33" s="45"/>
-      <c r="AC33" s="46"/>
-      <c r="AD33" s="46"/>
-      <c r="AE33" s="46"/>
-      <c r="AF33" s="46"/>
-      <c r="AG33" s="46"/>
-      <c r="AH33" s="46"/>
-      <c r="AI33" s="46"/>
-      <c r="AJ33" s="55"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+      <c r="AA33" s="33"/>
+      <c r="AB33" s="36"/>
+      <c r="AC33" s="37"/>
+      <c r="AD33" s="37"/>
+      <c r="AE33" s="37"/>
+      <c r="AF33" s="37"/>
+      <c r="AG33" s="37"/>
+      <c r="AH33" s="37"/>
+      <c r="AI33" s="37"/>
       <c r="AQ33" s="20"/>
       <c r="AR33" s="3"/>
       <c r="AS33" s="3"/>
@@ -4438,35 +4469,34 @@
       <c r="DK33" s="3"/>
     </row>
     <row r="34" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="54"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="57"/>
       <c r="T34" s="11"/>
       <c r="V34" s="18"/>
-      <c r="W34" s="34"/>
-      <c r="X34" s="34"/>
-      <c r="Y34" s="34"/>
-      <c r="Z34" s="34"/>
-      <c r="AA34" s="35"/>
-      <c r="AB34" s="45"/>
-      <c r="AC34" s="46"/>
-      <c r="AD34" s="46"/>
-      <c r="AE34" s="46"/>
-      <c r="AF34" s="46"/>
-      <c r="AG34" s="46"/>
-      <c r="AH34" s="46"/>
-      <c r="AI34" s="46"/>
-      <c r="AJ34" s="55"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+      <c r="AA34" s="33"/>
+      <c r="AB34" s="36"/>
+      <c r="AC34" s="37"/>
+      <c r="AD34" s="37"/>
+      <c r="AE34" s="37"/>
+      <c r="AF34" s="37"/>
+      <c r="AG34" s="37"/>
+      <c r="AH34" s="37"/>
+      <c r="AI34" s="37"/>
       <c r="AQ34" s="20"/>
       <c r="AR34" s="3"/>
       <c r="AS34" s="3"/>
@@ -4542,35 +4572,34 @@
       <c r="DK34" s="3"/>
     </row>
     <row r="35" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="54"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="57"/>
       <c r="T35" s="11"/>
       <c r="V35" s="18"/>
-      <c r="W35" s="34"/>
-      <c r="X35" s="34"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="34"/>
-      <c r="AA35" s="35"/>
-      <c r="AB35" s="45"/>
-      <c r="AC35" s="46"/>
-      <c r="AD35" s="46"/>
-      <c r="AE35" s="46"/>
-      <c r="AF35" s="46"/>
-      <c r="AG35" s="46"/>
-      <c r="AH35" s="46"/>
-      <c r="AI35" s="46"/>
-      <c r="AJ35" s="55"/>
+      <c r="W35" s="32"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="32"/>
+      <c r="AA35" s="33"/>
+      <c r="AB35" s="36"/>
+      <c r="AC35" s="37"/>
+      <c r="AD35" s="37"/>
+      <c r="AE35" s="37"/>
+      <c r="AF35" s="37"/>
+      <c r="AG35" s="37"/>
+      <c r="AH35" s="37"/>
+      <c r="AI35" s="37"/>
       <c r="AQ35" s="20"/>
       <c r="AR35" s="3"/>
       <c r="AS35" s="3"/>
@@ -4646,35 +4675,34 @@
       <c r="DK35" s="3"/>
     </row>
     <row r="36" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="54"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="57"/>
       <c r="T36" s="11"/>
       <c r="V36" s="18"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="35"/>
-      <c r="AB36" s="45"/>
-      <c r="AC36" s="46"/>
-      <c r="AD36" s="46"/>
-      <c r="AE36" s="46"/>
-      <c r="AF36" s="46"/>
-      <c r="AG36" s="46"/>
-      <c r="AH36" s="46"/>
-      <c r="AI36" s="46"/>
-      <c r="AJ36" s="55"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+      <c r="AA36" s="33"/>
+      <c r="AB36" s="36"/>
+      <c r="AC36" s="37"/>
+      <c r="AD36" s="37"/>
+      <c r="AE36" s="37"/>
+      <c r="AF36" s="37"/>
+      <c r="AG36" s="37"/>
+      <c r="AH36" s="37"/>
+      <c r="AI36" s="37"/>
       <c r="AQ36" s="20"/>
       <c r="AR36" s="3"/>
       <c r="AS36" s="3"/>
@@ -4750,35 +4778,34 @@
       <c r="DK36" s="3"/>
     </row>
     <row r="37" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="54"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="57"/>
       <c r="T37" s="11"/>
       <c r="V37" s="18"/>
-      <c r="W37" s="34"/>
-      <c r="X37" s="34"/>
-      <c r="Y37" s="34"/>
-      <c r="Z37" s="34"/>
-      <c r="AA37" s="35"/>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="46"/>
-      <c r="AD37" s="46"/>
-      <c r="AE37" s="46"/>
-      <c r="AF37" s="46"/>
-      <c r="AG37" s="46"/>
-      <c r="AH37" s="46"/>
-      <c r="AI37" s="46"/>
-      <c r="AJ37" s="55"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+      <c r="AA37" s="33"/>
+      <c r="AB37" s="36"/>
+      <c r="AC37" s="37"/>
+      <c r="AD37" s="37"/>
+      <c r="AE37" s="37"/>
+      <c r="AF37" s="37"/>
+      <c r="AG37" s="37"/>
+      <c r="AH37" s="37"/>
+      <c r="AI37" s="37"/>
       <c r="AQ37" s="20"/>
       <c r="AR37" s="3"/>
       <c r="AS37" s="3"/>
@@ -4854,35 +4881,34 @@
       <c r="DK37" s="3"/>
     </row>
     <row r="38" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="54"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="57"/>
       <c r="T38" s="11"/>
       <c r="V38" s="18"/>
-      <c r="W38" s="34"/>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="34"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="35"/>
-      <c r="AB38" s="45"/>
-      <c r="AC38" s="46"/>
-      <c r="AD38" s="46"/>
-      <c r="AE38" s="46"/>
-      <c r="AF38" s="46"/>
-      <c r="AG38" s="46"/>
-      <c r="AH38" s="46"/>
-      <c r="AI38" s="46"/>
-      <c r="AJ38" s="55"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="32"/>
+      <c r="Z38" s="32"/>
+      <c r="AA38" s="33"/>
+      <c r="AB38" s="36"/>
+      <c r="AC38" s="37"/>
+      <c r="AD38" s="37"/>
+      <c r="AE38" s="37"/>
+      <c r="AF38" s="37"/>
+      <c r="AG38" s="37"/>
+      <c r="AH38" s="37"/>
+      <c r="AI38" s="37"/>
       <c r="AQ38" s="20"/>
       <c r="AR38" s="3"/>
       <c r="AS38" s="3"/>
@@ -4958,35 +4984,34 @@
       <c r="DK38" s="3"/>
     </row>
     <row r="39" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="54"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="57"/>
       <c r="T39" s="11"/>
       <c r="V39" s="18"/>
-      <c r="W39" s="34"/>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="45"/>
-      <c r="AC39" s="46"/>
-      <c r="AD39" s="46"/>
-      <c r="AE39" s="46"/>
-      <c r="AF39" s="46"/>
-      <c r="AG39" s="46"/>
-      <c r="AH39" s="46"/>
-      <c r="AI39" s="46"/>
-      <c r="AJ39" s="55"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+      <c r="AA39" s="33"/>
+      <c r="AB39" s="36"/>
+      <c r="AC39" s="37"/>
+      <c r="AD39" s="37"/>
+      <c r="AE39" s="37"/>
+      <c r="AF39" s="37"/>
+      <c r="AG39" s="37"/>
+      <c r="AH39" s="37"/>
+      <c r="AI39" s="37"/>
       <c r="AQ39" s="20"/>
       <c r="AR39" s="3"/>
       <c r="AS39" s="3"/>
@@ -5062,35 +5087,34 @@
       <c r="DK39" s="3"/>
     </row>
     <row r="40" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="54"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="57"/>
       <c r="T40" s="11"/>
       <c r="V40" s="18"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="34"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="45"/>
-      <c r="AC40" s="46"/>
-      <c r="AD40" s="46"/>
-      <c r="AE40" s="46"/>
-      <c r="AF40" s="46"/>
-      <c r="AG40" s="46"/>
-      <c r="AH40" s="46"/>
-      <c r="AI40" s="46"/>
-      <c r="AJ40" s="55"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="37"/>
+      <c r="AD40" s="37"/>
+      <c r="AE40" s="37"/>
+      <c r="AF40" s="37"/>
+      <c r="AG40" s="37"/>
+      <c r="AH40" s="37"/>
+      <c r="AI40" s="37"/>
       <c r="AQ40" s="20"/>
       <c r="AR40" s="3"/>
       <c r="AS40" s="3"/>
@@ -5166,35 +5190,34 @@
       <c r="DK40" s="3"/>
     </row>
     <row r="41" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="54"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="57"/>
       <c r="T41" s="11"/>
       <c r="V41" s="18"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="45"/>
-      <c r="AC41" s="46"/>
-      <c r="AD41" s="46"/>
-      <c r="AE41" s="46"/>
-      <c r="AF41" s="46"/>
-      <c r="AG41" s="46"/>
-      <c r="AH41" s="46"/>
-      <c r="AI41" s="46"/>
-      <c r="AJ41" s="55"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+      <c r="AA41" s="33"/>
+      <c r="AB41" s="36"/>
+      <c r="AC41" s="37"/>
+      <c r="AD41" s="37"/>
+      <c r="AE41" s="37"/>
+      <c r="AF41" s="37"/>
+      <c r="AG41" s="37"/>
+      <c r="AH41" s="37"/>
+      <c r="AI41" s="37"/>
       <c r="AQ41" s="20"/>
       <c r="AR41" s="3"/>
       <c r="AS41" s="3"/>
@@ -5270,35 +5293,34 @@
       <c r="DK41" s="3"/>
     </row>
     <row r="42" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="54"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="57"/>
       <c r="T42" s="11"/>
       <c r="V42" s="18"/>
-      <c r="W42" s="34"/>
-      <c r="X42" s="34"/>
-      <c r="Y42" s="34"/>
-      <c r="Z42" s="34"/>
-      <c r="AA42" s="35"/>
-      <c r="AB42" s="45"/>
-      <c r="AC42" s="46"/>
-      <c r="AD42" s="46"/>
-      <c r="AE42" s="46"/>
-      <c r="AF42" s="46"/>
-      <c r="AG42" s="46"/>
-      <c r="AH42" s="46"/>
-      <c r="AI42" s="46"/>
-      <c r="AJ42" s="55"/>
+      <c r="W42" s="32"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="32"/>
+      <c r="Z42" s="32"/>
+      <c r="AA42" s="33"/>
+      <c r="AB42" s="36"/>
+      <c r="AC42" s="37"/>
+      <c r="AD42" s="37"/>
+      <c r="AE42" s="37"/>
+      <c r="AF42" s="37"/>
+      <c r="AG42" s="37"/>
+      <c r="AH42" s="37"/>
+      <c r="AI42" s="37"/>
       <c r="AQ42" s="20"/>
       <c r="AR42" s="3"/>
       <c r="AS42" s="3"/>
@@ -5374,35 +5396,34 @@
       <c r="DK42" s="3"/>
     </row>
     <row r="43" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="52"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="54"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="37"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="57"/>
       <c r="T43" s="11"/>
       <c r="V43" s="18"/>
-      <c r="W43" s="34"/>
-      <c r="X43" s="34"/>
-      <c r="Y43" s="34"/>
-      <c r="Z43" s="34"/>
-      <c r="AA43" s="35"/>
-      <c r="AB43" s="45"/>
-      <c r="AC43" s="46"/>
-      <c r="AD43" s="46"/>
-      <c r="AE43" s="46"/>
-      <c r="AF43" s="46"/>
-      <c r="AG43" s="46"/>
-      <c r="AH43" s="46"/>
-      <c r="AI43" s="46"/>
-      <c r="AJ43" s="55"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
+      <c r="Z43" s="32"/>
+      <c r="AA43" s="33"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="37"/>
+      <c r="AD43" s="37"/>
+      <c r="AE43" s="37"/>
+      <c r="AF43" s="37"/>
+      <c r="AG43" s="37"/>
+      <c r="AH43" s="37"/>
+      <c r="AI43" s="37"/>
       <c r="AQ43" s="20"/>
       <c r="AR43" s="3"/>
       <c r="AS43" s="3"/>
@@ -5478,35 +5499,34 @@
       <c r="DK43" s="3"/>
     </row>
     <row r="44" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="54"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="57"/>
       <c r="T44" s="11"/>
       <c r="V44" s="18"/>
-      <c r="W44" s="34"/>
-      <c r="X44" s="34"/>
-      <c r="Y44" s="34"/>
-      <c r="Z44" s="34"/>
-      <c r="AA44" s="35"/>
-      <c r="AB44" s="45"/>
-      <c r="AC44" s="46"/>
-      <c r="AD44" s="46"/>
-      <c r="AE44" s="46"/>
-      <c r="AF44" s="46"/>
-      <c r="AG44" s="46"/>
-      <c r="AH44" s="46"/>
-      <c r="AI44" s="46"/>
-      <c r="AJ44" s="55"/>
+      <c r="W44" s="32"/>
+      <c r="X44" s="32"/>
+      <c r="Y44" s="32"/>
+      <c r="Z44" s="32"/>
+      <c r="AA44" s="33"/>
+      <c r="AB44" s="36"/>
+      <c r="AC44" s="37"/>
+      <c r="AD44" s="37"/>
+      <c r="AE44" s="37"/>
+      <c r="AF44" s="37"/>
+      <c r="AG44" s="37"/>
+      <c r="AH44" s="37"/>
+      <c r="AI44" s="37"/>
       <c r="AQ44" s="20"/>
       <c r="AR44" s="3"/>
       <c r="AS44" s="3"/>
@@ -5582,35 +5602,34 @@
       <c r="DK44" s="3"/>
     </row>
     <row r="45" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="54"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="57"/>
       <c r="T45" s="11"/>
       <c r="V45" s="18"/>
-      <c r="W45" s="34"/>
-      <c r="X45" s="34"/>
-      <c r="Y45" s="34"/>
-      <c r="Z45" s="34"/>
-      <c r="AA45" s="35"/>
-      <c r="AB45" s="45"/>
-      <c r="AC45" s="46"/>
-      <c r="AD45" s="46"/>
-      <c r="AE45" s="46"/>
-      <c r="AF45" s="46"/>
-      <c r="AG45" s="46"/>
-      <c r="AH45" s="46"/>
-      <c r="AI45" s="46"/>
-      <c r="AJ45" s="55"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="32"/>
+      <c r="Z45" s="32"/>
+      <c r="AA45" s="33"/>
+      <c r="AB45" s="36"/>
+      <c r="AC45" s="37"/>
+      <c r="AD45" s="37"/>
+      <c r="AE45" s="37"/>
+      <c r="AF45" s="37"/>
+      <c r="AG45" s="37"/>
+      <c r="AH45" s="37"/>
+      <c r="AI45" s="37"/>
       <c r="AQ45" s="20"/>
       <c r="AR45" s="3"/>
       <c r="AS45" s="3"/>
@@ -5686,35 +5705,34 @@
       <c r="DK45" s="3"/>
     </row>
     <row r="46" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="53"/>
-      <c r="M46" s="54"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="57"/>
       <c r="T46" s="11"/>
       <c r="V46" s="20"/>
-      <c r="W46" s="34"/>
-      <c r="X46" s="34"/>
-      <c r="Y46" s="34"/>
-      <c r="Z46" s="34"/>
-      <c r="AA46" s="35"/>
-      <c r="AB46" s="45"/>
-      <c r="AC46" s="46"/>
-      <c r="AD46" s="46"/>
-      <c r="AE46" s="46"/>
-      <c r="AF46" s="46"/>
-      <c r="AG46" s="46"/>
-      <c r="AH46" s="46"/>
-      <c r="AI46" s="46"/>
-      <c r="AJ46" s="55"/>
+      <c r="W46" s="32"/>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="32"/>
+      <c r="Z46" s="32"/>
+      <c r="AA46" s="33"/>
+      <c r="AB46" s="36"/>
+      <c r="AC46" s="37"/>
+      <c r="AD46" s="37"/>
+      <c r="AE46" s="37"/>
+      <c r="AF46" s="37"/>
+      <c r="AG46" s="37"/>
+      <c r="AH46" s="37"/>
+      <c r="AI46" s="37"/>
       <c r="AQ46" s="20"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
@@ -5790,35 +5808,34 @@
       <c r="DK46" s="3"/>
     </row>
     <row r="47" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="54"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="57"/>
       <c r="T47" s="11"/>
       <c r="V47" s="11"/>
-      <c r="W47" s="34"/>
-      <c r="X47" s="34"/>
-      <c r="Y47" s="34"/>
-      <c r="Z47" s="34"/>
-      <c r="AA47" s="35"/>
-      <c r="AB47" s="45"/>
-      <c r="AC47" s="46"/>
-      <c r="AD47" s="46"/>
-      <c r="AE47" s="46"/>
-      <c r="AF47" s="46"/>
-      <c r="AG47" s="46"/>
-      <c r="AH47" s="46"/>
-      <c r="AI47" s="46"/>
-      <c r="AJ47" s="55"/>
+      <c r="W47" s="32"/>
+      <c r="X47" s="32"/>
+      <c r="Y47" s="32"/>
+      <c r="Z47" s="32"/>
+      <c r="AA47" s="33"/>
+      <c r="AB47" s="36"/>
+      <c r="AC47" s="37"/>
+      <c r="AD47" s="37"/>
+      <c r="AE47" s="37"/>
+      <c r="AF47" s="37"/>
+      <c r="AG47" s="37"/>
+      <c r="AH47" s="37"/>
+      <c r="AI47" s="37"/>
       <c r="AQ47" s="20"/>
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
@@ -5894,35 +5911,35 @@
       <c r="DK47" s="3"/>
     </row>
     <row r="48" spans="1:115" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="54"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="57"/>
       <c r="T48" s="11"/>
       <c r="V48" s="11"/>
-      <c r="W48" s="34"/>
-      <c r="X48" s="34"/>
-      <c r="Y48" s="34"/>
-      <c r="Z48" s="34"/>
-      <c r="AA48" s="35"/>
-      <c r="AB48" s="45"/>
-      <c r="AC48" s="46"/>
-      <c r="AD48" s="46"/>
-      <c r="AE48" s="46"/>
-      <c r="AF48" s="46"/>
-      <c r="AG48" s="46"/>
-      <c r="AH48" s="46"/>
-      <c r="AI48" s="46"/>
-      <c r="AJ48" s="55"/>
+      <c r="W48" s="32"/>
+      <c r="X48" s="32"/>
+      <c r="Y48" s="32"/>
+      <c r="Z48" s="32"/>
+      <c r="AA48" s="33"/>
+      <c r="AB48" s="36"/>
+      <c r="AC48" s="37"/>
+      <c r="AD48" s="37"/>
+      <c r="AE48" s="37"/>
+      <c r="AF48" s="37"/>
+      <c r="AG48" s="37"/>
+      <c r="AH48" s="37"/>
+      <c r="AI48" s="37"/>
+      <c r="AQ48" s="11"/>
       <c r="AR48" s="3"/>
       <c r="AS48" s="3"/>
       <c r="AT48" s="3"/>
@@ -5997,53 +6014,53 @@
       <c r="DK48" s="3"/>
     </row>
     <row r="49" spans="1:115" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="33"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
-      <c r="R49" s="33"/>
-      <c r="S49" s="33"/>
-      <c r="T49" s="33"/>
-      <c r="U49" s="33"/>
-      <c r="V49" s="33" t="s">
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
+      <c r="R49" s="56"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
+      <c r="V49" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="W49" s="33"/>
-      <c r="X49" s="33"/>
-      <c r="Y49" s="33"/>
-      <c r="Z49" s="33"/>
-      <c r="AA49" s="33"/>
-      <c r="AB49" s="33"/>
-      <c r="AC49" s="33"/>
-      <c r="AD49" s="33"/>
-      <c r="AE49" s="33"/>
-      <c r="AF49" s="33"/>
-      <c r="AG49" s="33"/>
-      <c r="AH49" s="33"/>
-      <c r="AI49" s="33"/>
-      <c r="AJ49" s="33"/>
-      <c r="AK49" s="33"/>
-      <c r="AL49" s="33"/>
-      <c r="AM49" s="33"/>
-      <c r="AN49" s="33"/>
-      <c r="AO49" s="33"/>
-      <c r="AP49" s="33"/>
-      <c r="AQ49" s="33"/>
+      <c r="W49" s="56"/>
+      <c r="X49" s="56"/>
+      <c r="Y49" s="56"/>
+      <c r="Z49" s="56"/>
+      <c r="AA49" s="56"/>
+      <c r="AB49" s="56"/>
+      <c r="AC49" s="56"/>
+      <c r="AD49" s="56"/>
+      <c r="AE49" s="56"/>
+      <c r="AF49" s="56"/>
+      <c r="AG49" s="56"/>
+      <c r="AH49" s="56"/>
+      <c r="AI49" s="56"/>
+      <c r="AJ49" s="56"/>
+      <c r="AK49" s="56"/>
+      <c r="AL49" s="56"/>
+      <c r="AM49" s="56"/>
+      <c r="AN49" s="56"/>
+      <c r="AO49" s="56"/>
+      <c r="AP49" s="56"/>
+      <c r="AQ49" s="56"/>
       <c r="AR49" s="3"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
@@ -6138,7 +6155,7 @@
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
-      <c r="U50" s="27"/>
+      <c r="U50" s="25"/>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
@@ -6255,7 +6272,7 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
-      <c r="U51" s="27"/>
+      <c r="U51" s="25"/>
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
@@ -6300,7 +6317,7 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
-      <c r="U52" s="27"/>
+      <c r="U52" s="25"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
@@ -6417,7 +6434,7 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
-      <c r="U53" s="27"/>
+      <c r="U53" s="25"/>
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
@@ -6534,7 +6551,7 @@
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
-      <c r="U54" s="27"/>
+      <c r="U54" s="25"/>
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
@@ -6651,7 +6668,7 @@
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
-      <c r="U55" s="27"/>
+      <c r="U55" s="25"/>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
@@ -6768,7 +6785,7 @@
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
-      <c r="U56" s="27"/>
+      <c r="U56" s="25"/>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
@@ -6885,7 +6902,7 @@
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
-      <c r="U57" s="27"/>
+      <c r="U57" s="25"/>
       <c r="V57" s="3"/>
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
@@ -7002,7 +7019,7 @@
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
-      <c r="U58" s="28"/>
+      <c r="U58" s="26"/>
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
@@ -7119,7 +7136,7 @@
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
-      <c r="U59" s="28"/>
+      <c r="U59" s="26"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
@@ -7236,7 +7253,7 @@
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
-      <c r="U60" s="28"/>
+      <c r="U60" s="26"/>
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
       <c r="X60" s="2"/>
@@ -7353,7 +7370,7 @@
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-      <c r="U61" s="28"/>
+      <c r="U61" s="26"/>
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
@@ -7470,7 +7487,7 @@
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
-      <c r="U62" s="28"/>
+      <c r="U62" s="26"/>
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
       <c r="X62" s="2"/>
@@ -7587,7 +7604,7 @@
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
-      <c r="U63" s="28"/>
+      <c r="U63" s="26"/>
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
       <c r="X63" s="2"/>
@@ -7704,7 +7721,7 @@
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
-      <c r="U64" s="28"/>
+      <c r="U64" s="26"/>
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
       <c r="X64" s="2"/>
@@ -7821,7 +7838,7 @@
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
-      <c r="U65" s="28"/>
+      <c r="U65" s="26"/>
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
       <c r="X65" s="2"/>
@@ -7938,7 +7955,7 @@
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
-      <c r="U66" s="28"/>
+      <c r="U66" s="26"/>
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
@@ -8055,7 +8072,7 @@
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
-      <c r="U67" s="28"/>
+      <c r="U67" s="26"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
@@ -8172,7 +8189,7 @@
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
-      <c r="U68" s="28"/>
+      <c r="U68" s="26"/>
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
@@ -8289,7 +8306,7 @@
       <c r="R69" s="2"/>
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
-      <c r="U69" s="28"/>
+      <c r="U69" s="26"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
       <c r="X69" s="2"/>
@@ -8406,7 +8423,7 @@
       <c r="R70" s="2"/>
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
-      <c r="U70" s="28"/>
+      <c r="U70" s="26"/>
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
       <c r="X70" s="2"/>
@@ -8523,7 +8540,7 @@
       <c r="R71" s="2"/>
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
-      <c r="U71" s="28"/>
+      <c r="U71" s="26"/>
       <c r="V71" s="2"/>
       <c r="W71" s="2"/>
       <c r="X71" s="2"/>
@@ -8640,7 +8657,7 @@
       <c r="R72" s="2"/>
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
-      <c r="U72" s="28"/>
+      <c r="U72" s="26"/>
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
@@ -8757,7 +8774,7 @@
       <c r="R73" s="2"/>
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
-      <c r="U73" s="28"/>
+      <c r="U73" s="26"/>
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
       <c r="X73" s="2"/>
@@ -8874,7 +8891,7 @@
       <c r="R74" s="2"/>
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
-      <c r="U74" s="28"/>
+      <c r="U74" s="26"/>
       <c r="V74" s="2"/>
       <c r="W74" s="2"/>
       <c r="X74" s="2"/>
@@ -8991,7 +9008,7 @@
       <c r="R75" s="2"/>
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
-      <c r="U75" s="28"/>
+      <c r="U75" s="26"/>
       <c r="V75" s="2"/>
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
@@ -9108,7 +9125,7 @@
       <c r="R76" s="2"/>
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
-      <c r="U76" s="28"/>
+      <c r="U76" s="26"/>
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
       <c r="X76" s="2"/>
@@ -9225,7 +9242,7 @@
       <c r="R77" s="2"/>
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
-      <c r="U77" s="28"/>
+      <c r="U77" s="26"/>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
@@ -9342,7 +9359,7 @@
       <c r="R78" s="2"/>
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
-      <c r="U78" s="28"/>
+      <c r="U78" s="26"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
       <c r="X78" s="2"/>
@@ -9459,7 +9476,7 @@
       <c r="R79" s="2"/>
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
-      <c r="U79" s="28"/>
+      <c r="U79" s="26"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
@@ -9576,7 +9593,7 @@
       <c r="R80" s="2"/>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
-      <c r="U80" s="28"/>
+      <c r="U80" s="26"/>
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
       <c r="X80" s="2"/>
@@ -9693,7 +9710,7 @@
       <c r="R81" s="2"/>
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
-      <c r="U81" s="28"/>
+      <c r="U81" s="26"/>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
@@ -9810,7 +9827,7 @@
       <c r="R82" s="2"/>
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
-      <c r="U82" s="28"/>
+      <c r="U82" s="26"/>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
       <c r="X82" s="2"/>
@@ -9927,7 +9944,7 @@
       <c r="R83" s="2"/>
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
-      <c r="U83" s="28"/>
+      <c r="U83" s="26"/>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
       <c r="X83" s="2"/>
@@ -10044,7 +10061,7 @@
       <c r="R84" s="2"/>
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
-      <c r="U84" s="28"/>
+      <c r="U84" s="26"/>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
       <c r="X84" s="2"/>
@@ -10161,7 +10178,7 @@
       <c r="R85" s="2"/>
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
-      <c r="U85" s="28"/>
+      <c r="U85" s="26"/>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
       <c r="X85" s="2"/>
@@ -10278,7 +10295,7 @@
       <c r="R86" s="2"/>
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
-      <c r="U86" s="28"/>
+      <c r="U86" s="26"/>
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
       <c r="X86" s="2"/>
@@ -10395,7 +10412,7 @@
       <c r="R87" s="2"/>
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
-      <c r="U87" s="28"/>
+      <c r="U87" s="26"/>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
       <c r="X87" s="2"/>
@@ -10512,7 +10529,7 @@
       <c r="R88" s="2"/>
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
-      <c r="U88" s="28"/>
+      <c r="U88" s="26"/>
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
       <c r="X88" s="2"/>
@@ -10629,7 +10646,7 @@
       <c r="R89" s="2"/>
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
-      <c r="U89" s="28"/>
+      <c r="U89" s="26"/>
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
       <c r="X89" s="2"/>
@@ -10746,7 +10763,7 @@
       <c r="R90" s="2"/>
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
-      <c r="U90" s="28"/>
+      <c r="U90" s="26"/>
       <c r="V90" s="2"/>
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
@@ -10863,7 +10880,7 @@
       <c r="R91" s="2"/>
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
-      <c r="U91" s="28"/>
+      <c r="U91" s="26"/>
       <c r="V91" s="2"/>
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
@@ -10980,7 +10997,7 @@
       <c r="R92" s="2"/>
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
-      <c r="U92" s="28"/>
+      <c r="U92" s="26"/>
       <c r="V92" s="2"/>
       <c r="W92" s="2"/>
       <c r="X92" s="2"/>
@@ -11097,7 +11114,7 @@
       <c r="R93" s="2"/>
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
-      <c r="U93" s="28"/>
+      <c r="U93" s="26"/>
       <c r="V93" s="2"/>
       <c r="W93" s="2"/>
       <c r="X93" s="2"/>
@@ -11214,7 +11231,7 @@
       <c r="R94" s="2"/>
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
-      <c r="U94" s="28"/>
+      <c r="U94" s="26"/>
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
       <c r="X94" s="2"/>
@@ -11331,7 +11348,7 @@
       <c r="R95" s="2"/>
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
-      <c r="U95" s="28"/>
+      <c r="U95" s="26"/>
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
       <c r="X95" s="2"/>
@@ -11448,7 +11465,7 @@
       <c r="R96" s="2"/>
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
-      <c r="U96" s="28"/>
+      <c r="U96" s="26"/>
       <c r="V96" s="2"/>
       <c r="W96" s="2"/>
       <c r="X96" s="2"/>
@@ -11565,7 +11582,7 @@
       <c r="R97" s="2"/>
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
-      <c r="U97" s="28"/>
+      <c r="U97" s="26"/>
       <c r="V97" s="2"/>
       <c r="W97" s="2"/>
       <c r="X97" s="2"/>
@@ -11682,7 +11699,7 @@
       <c r="R98" s="2"/>
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
-      <c r="U98" s="28"/>
+      <c r="U98" s="26"/>
       <c r="V98" s="2"/>
       <c r="W98" s="2"/>
       <c r="X98" s="2"/>
@@ -11799,7 +11816,7 @@
       <c r="R99" s="2"/>
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
-      <c r="U99" s="28"/>
+      <c r="U99" s="26"/>
       <c r="V99" s="2"/>
       <c r="W99" s="2"/>
       <c r="X99" s="2"/>
@@ -11844,7 +11861,7 @@
       <c r="R100" s="2"/>
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
-      <c r="U100" s="28"/>
+      <c r="U100" s="26"/>
       <c r="V100" s="2"/>
       <c r="W100" s="2"/>
       <c r="X100" s="2"/>
@@ -11889,7 +11906,7 @@
       <c r="R101" s="2"/>
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
-      <c r="U101" s="28"/>
+      <c r="U101" s="26"/>
       <c r="V101" s="2"/>
       <c r="W101" s="2"/>
       <c r="X101" s="2"/>
@@ -11934,7 +11951,7 @@
       <c r="R102" s="2"/>
       <c r="S102" s="2"/>
       <c r="T102" s="2"/>
-      <c r="U102" s="28"/>
+      <c r="U102" s="26"/>
       <c r="V102" s="2"/>
       <c r="W102" s="2"/>
       <c r="X102" s="2"/>
@@ -11979,7 +11996,7 @@
       <c r="R103" s="2"/>
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
-      <c r="U103" s="28"/>
+      <c r="U103" s="26"/>
       <c r="V103" s="2"/>
       <c r="W103" s="2"/>
       <c r="X103" s="2"/>
@@ -12024,7 +12041,7 @@
       <c r="R104" s="2"/>
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
-      <c r="U104" s="28"/>
+      <c r="U104" s="26"/>
       <c r="V104" s="2"/>
       <c r="W104" s="2"/>
       <c r="X104" s="2"/>
@@ -12069,7 +12086,7 @@
       <c r="R105" s="2"/>
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
-      <c r="U105" s="28"/>
+      <c r="U105" s="26"/>
       <c r="V105" s="2"/>
       <c r="W105" s="2"/>
       <c r="X105" s="2"/>
@@ -12114,7 +12131,7 @@
       <c r="R106" s="2"/>
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
-      <c r="U106" s="28"/>
+      <c r="U106" s="26"/>
       <c r="V106" s="2"/>
       <c r="W106" s="2"/>
       <c r="X106" s="2"/>
@@ -12139,9 +12156,25 @@
       <c r="AQ106" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="192">
-    <mergeCell ref="AB48:AI48"/>
-    <mergeCell ref="AB6:AI6"/>
+  <mergeCells count="196">
+    <mergeCell ref="W35:AA35"/>
+    <mergeCell ref="W36:AA36"/>
+    <mergeCell ref="W37:AA37"/>
+    <mergeCell ref="W26:AA26"/>
+    <mergeCell ref="W27:AA27"/>
+    <mergeCell ref="W28:AA28"/>
+    <mergeCell ref="W38:AA38"/>
+    <mergeCell ref="W39:AA39"/>
+    <mergeCell ref="W40:AA40"/>
+    <mergeCell ref="AB20:AI20"/>
+    <mergeCell ref="AB21:AI21"/>
+    <mergeCell ref="AB22:AI22"/>
+    <mergeCell ref="AB23:AI23"/>
+    <mergeCell ref="AB24:AI24"/>
+    <mergeCell ref="AB25:AI25"/>
+    <mergeCell ref="AB26:AI26"/>
+    <mergeCell ref="AB27:AI27"/>
+    <mergeCell ref="AB28:AI28"/>
     <mergeCell ref="AB32:AI32"/>
     <mergeCell ref="AB33:AI33"/>
     <mergeCell ref="AB34:AI34"/>
@@ -12151,35 +12184,9 @@
     <mergeCell ref="AB38:AI38"/>
     <mergeCell ref="AB39:AI39"/>
     <mergeCell ref="AB40:AI40"/>
-    <mergeCell ref="AB7:AI7"/>
-    <mergeCell ref="AB8:AI8"/>
-    <mergeCell ref="AB9:AI9"/>
-    <mergeCell ref="AB10:AI10"/>
-    <mergeCell ref="AB11:AI11"/>
-    <mergeCell ref="AB12:AI12"/>
-    <mergeCell ref="AB13:AI13"/>
-    <mergeCell ref="AB14:AI14"/>
-    <mergeCell ref="AB15:AI15"/>
-    <mergeCell ref="AB16:AI16"/>
-    <mergeCell ref="AB17:AI17"/>
-    <mergeCell ref="AB18:AI18"/>
-    <mergeCell ref="AB19:AI19"/>
-    <mergeCell ref="AB20:AI20"/>
-    <mergeCell ref="AB21:AI21"/>
-    <mergeCell ref="AB22:AI22"/>
-    <mergeCell ref="AB23:AI23"/>
-    <mergeCell ref="AB24:AI24"/>
-    <mergeCell ref="AB25:AI25"/>
-    <mergeCell ref="AB26:AI26"/>
-    <mergeCell ref="AB27:AI27"/>
-    <mergeCell ref="AB28:AI28"/>
-    <mergeCell ref="AB41:AI41"/>
-    <mergeCell ref="AB42:AI42"/>
-    <mergeCell ref="AB43:AI43"/>
-    <mergeCell ref="AB44:AI44"/>
-    <mergeCell ref="AB45:AI45"/>
-    <mergeCell ref="AB46:AI46"/>
-    <mergeCell ref="AB47:AI47"/>
+    <mergeCell ref="W23:AA23"/>
+    <mergeCell ref="W24:AA24"/>
+    <mergeCell ref="W25:AA25"/>
     <mergeCell ref="F35:M35"/>
     <mergeCell ref="F36:M36"/>
     <mergeCell ref="F37:M37"/>
@@ -12198,6 +12205,13 @@
     <mergeCell ref="F26:M26"/>
     <mergeCell ref="F27:M27"/>
     <mergeCell ref="F28:M28"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A44:E44"/>
     <mergeCell ref="AB29:AI29"/>
     <mergeCell ref="AB30:AI30"/>
     <mergeCell ref="AB31:AI31"/>
@@ -12207,15 +12221,17 @@
     <mergeCell ref="F32:M32"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="F34:M34"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="W29:AA29"/>
+    <mergeCell ref="W30:AA30"/>
+    <mergeCell ref="W31:AA31"/>
+    <mergeCell ref="W32:AA32"/>
+    <mergeCell ref="W33:AA33"/>
+    <mergeCell ref="W34:AA34"/>
+    <mergeCell ref="AB41:AI41"/>
+    <mergeCell ref="AB42:AI42"/>
+    <mergeCell ref="F17:M17"/>
+    <mergeCell ref="F18:M18"/>
+    <mergeCell ref="F19:M19"/>
     <mergeCell ref="A45:E45"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A19:E19"/>
@@ -12235,15 +12251,8 @@
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A34:E34"/>
-    <mergeCell ref="W20:AA20"/>
-    <mergeCell ref="W21:AA21"/>
-    <mergeCell ref="W22:AA22"/>
-    <mergeCell ref="W11:AA11"/>
-    <mergeCell ref="W12:AA12"/>
-    <mergeCell ref="W13:AA13"/>
-    <mergeCell ref="W14:AA14"/>
-    <mergeCell ref="W15:AA15"/>
-    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
@@ -12256,12 +12265,6 @@
     <mergeCell ref="F15:M15"/>
     <mergeCell ref="F14:M14"/>
     <mergeCell ref="F16:M16"/>
-    <mergeCell ref="F17:M17"/>
-    <mergeCell ref="F18:M18"/>
-    <mergeCell ref="F19:M19"/>
-    <mergeCell ref="W8:AA8"/>
-    <mergeCell ref="W9:AA9"/>
-    <mergeCell ref="W10:AA10"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A5:E5"/>
@@ -12277,6 +12280,15 @@
     <mergeCell ref="F10:M10"/>
     <mergeCell ref="F9:M9"/>
     <mergeCell ref="F6:M6"/>
+    <mergeCell ref="V4:AA4"/>
+    <mergeCell ref="V5:AA5"/>
+    <mergeCell ref="W16:AA16"/>
+    <mergeCell ref="W11:AA11"/>
+    <mergeCell ref="W12:AA12"/>
+    <mergeCell ref="W13:AA13"/>
+    <mergeCell ref="W14:AA14"/>
+    <mergeCell ref="W15:AA15"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A49:U49"/>
     <mergeCell ref="W47:AA47"/>
     <mergeCell ref="W48:AA48"/>
@@ -12294,6 +12306,15 @@
     <mergeCell ref="F46:M46"/>
     <mergeCell ref="F47:M47"/>
     <mergeCell ref="F48:M48"/>
+    <mergeCell ref="V49:AQ49"/>
+    <mergeCell ref="AB43:AI43"/>
+    <mergeCell ref="AB44:AI44"/>
+    <mergeCell ref="AB45:AI45"/>
+    <mergeCell ref="AB46:AI46"/>
+    <mergeCell ref="AB47:AI47"/>
+    <mergeCell ref="AB48:AI48"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="F5:M5"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AJ1"/>
@@ -12308,30 +12329,30 @@
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="V2:AQ3"/>
-    <mergeCell ref="V4:AA4"/>
-    <mergeCell ref="V5:AA5"/>
-    <mergeCell ref="V49:AQ49"/>
-    <mergeCell ref="W35:AA35"/>
-    <mergeCell ref="W36:AA36"/>
-    <mergeCell ref="W37:AA37"/>
-    <mergeCell ref="W38:AA38"/>
-    <mergeCell ref="W39:AA39"/>
-    <mergeCell ref="W40:AA40"/>
-    <mergeCell ref="W29:AA29"/>
-    <mergeCell ref="W16:AA16"/>
-    <mergeCell ref="W30:AA30"/>
-    <mergeCell ref="W31:AA31"/>
-    <mergeCell ref="W32:AA32"/>
-    <mergeCell ref="W33:AA33"/>
-    <mergeCell ref="W34:AA34"/>
-    <mergeCell ref="W23:AA23"/>
-    <mergeCell ref="W24:AA24"/>
-    <mergeCell ref="W25:AA25"/>
-    <mergeCell ref="W26:AA26"/>
-    <mergeCell ref="W27:AA27"/>
-    <mergeCell ref="W28:AA28"/>
+    <mergeCell ref="AB5:AI5"/>
+    <mergeCell ref="AB4:AI4"/>
     <mergeCell ref="W6:AA6"/>
     <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="W8:AA8"/>
+    <mergeCell ref="W9:AA9"/>
+    <mergeCell ref="W10:AA10"/>
+    <mergeCell ref="W20:AA20"/>
+    <mergeCell ref="W21:AA21"/>
+    <mergeCell ref="W22:AA22"/>
+    <mergeCell ref="AB6:AI6"/>
+    <mergeCell ref="AB7:AI7"/>
+    <mergeCell ref="AB8:AI8"/>
+    <mergeCell ref="AB9:AI9"/>
+    <mergeCell ref="AB10:AI10"/>
+    <mergeCell ref="AB11:AI11"/>
+    <mergeCell ref="AB12:AI12"/>
+    <mergeCell ref="AB13:AI13"/>
+    <mergeCell ref="AB14:AI14"/>
+    <mergeCell ref="AB15:AI15"/>
+    <mergeCell ref="AB16:AI16"/>
+    <mergeCell ref="AB17:AI17"/>
+    <mergeCell ref="AB18:AI18"/>
+    <mergeCell ref="AB19:AI19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>